<commit_message>
xlxs update (fialed aproach no enought dat in xlxs will generate our own)
</commit_message>
<xml_diff>
--- a/XSLTapi/resources/ReleaseNotes-002.xlsx
+++ b/XSLTapi/resources/ReleaseNotes-002.xlsx
@@ -28,6 +28,34 @@
   </authors>
   <commentList>
     <comment ref="G3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>Sulek, Martin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t xml:space="preserve">
+New - new global variable
+Update - updated global variable
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="228">
   <si>
     <t>Relys2</t>
   </si>
@@ -907,7 +935,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -926,12 +954,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,8 +967,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1412,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,34 +1473,36 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="18" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="16" t="s">
         <v>66</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="19"/>
+      <c r="G4" s="16" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -1849,16 +1876,16 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+    <row r="50" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="12" t="s">
+    <row r="51" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="10" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1878,28 +1905,28 @@
         <v>17030</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
+    <row r="54" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="J54" s="13" t="s">
+      <c r="J54" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="K54" s="14" t="s">
+      <c r="K54" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="L54" s="14" t="s">
+      <c r="L54" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="M54" s="13" t="s">
+      <c r="M54" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="12" t="s">
+    <row r="55" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I55" s="12" t="s">
+      <c r="I55" s="10" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1976,8 +2003,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+    <row r="62" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="10" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2001,21 +2028,21 @@
       <c r="J65" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K65" s="15" t="s">
+      <c r="K65" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="L65" s="15" t="s">
+      <c r="L65" s="13" t="s">
         <v>75</v>
       </c>
       <c r="M65" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="2:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="12" t="s">
+    <row r="66" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I66" s="12" t="s">
+      <c r="I66" s="10" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2072,8 +2099,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="2:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="12" t="s">
+    <row r="72" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="10" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2097,21 +2124,21 @@
       <c r="J75" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K75" s="15" t="s">
+      <c r="K75" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="L75" s="15" t="s">
+      <c r="L75" s="13" t="s">
         <v>75</v>
       </c>
       <c r="M75" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="2:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="12" t="s">
+    <row r="76" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I76" s="12" t="s">
+      <c r="I76" s="10" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2156,9 +2183,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G3:G4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -2327,14 +2351,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="18"/>
       <c r="E7" t="s">
         <v>25</v>
       </c>
@@ -2881,7 +2905,7 @@
       <c r="B1" t="s">
         <v>214</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>